<commit_message>
add Event Module TestCases
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/EmployeeRewardSysTestData.xlsx
+++ b/src/main/java/com/qa/testdata/EmployeeRewardSysTestData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mygoa\Desktop\java\seleniumDemo\QA\SeleniumWorkSpace\com.EmployeeRewardSystemTest\src\main\java\com\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mygoa\Desktop\java\My_Project\git\com.EmployeeRewardSystemTest\src\main\java\com\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775233E5-ED2A-4912-BB07-ECAB307BDB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98C070C-993E-4EB2-B11B-CC1141095105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{53C2A3DE-A7C0-4FD4-A1B3-433E94FE1ECE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{53C2A3DE-A7C0-4FD4-A1B3-433E94FE1ECE}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
-    <sheet name="Reward" sheetId="2" r:id="rId2"/>
-    <sheet name="Role" sheetId="3" r:id="rId3"/>
+    <sheet name="Events" sheetId="4" r:id="rId2"/>
+    <sheet name="Reward" sheetId="2" r:id="rId3"/>
+    <sheet name="Role" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Rewa</t>
   </si>
@@ -161,6 +162,30 @@
   </si>
   <si>
     <t>1986-03-23</t>
+  </si>
+  <si>
+    <t>eventname</t>
+  </si>
+  <si>
+    <t>eventdescription</t>
+  </si>
+  <si>
+    <t>eventdocument</t>
+  </si>
+  <si>
+    <t>code ninjas</t>
+  </si>
+  <si>
+    <t>hacker throne</t>
+  </si>
+  <si>
+    <t>Have a blast building awesome video games and developing ninja coding skills on the path from white to black belt.</t>
+  </si>
+  <si>
+    <t>A hackathon is a fast-paced collaborative event lasting 24-48 hours where people work on engineering projects.</t>
+  </si>
+  <si>
+    <t>C:/Users/mygoa/Pictures/codeNinjas.png</t>
   </si>
 </sst>
 </file>
@@ -533,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A12BD1C-3294-49F8-8BC6-81D5D5B80F8D}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -711,6 +736,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E905269C-FD12-461A-8E88-01BD361E7031}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="94.109375" customWidth="1"/>
+    <col min="3" max="3" width="35.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CF802D-52B5-420F-AAFA-68C075807D0B}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -728,7 +806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A798D985-7649-4433-A7E9-EAD7C3988FC8}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>